<commit_message>
added fix for #REF! and other DB Func problems added fix for orphaned DBFunctions fixed DBAddinSetting extraction at end updated documentation
</commit_message>
<xml_diff>
--- a/test/DBSetQueryTests.xlsx
+++ b/test/DBSetQueryTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288F1B93-1DC0-4BA5-8EFD-8263A433760B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFBEDE4-87C1-479B-A1B8-E70EC78C9FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConnSetting" sheetId="2" r:id="rId1"/>
@@ -24,23 +24,22 @@
     <definedName name="DBFsource0d6e4daa4bc1480498245f08c4eb094b" hidden="1">'1'!$A$3</definedName>
     <definedName name="DBFsource663f4cc231bd4c42bd757fd9e6d2c563" hidden="1">'3'!$B$19</definedName>
     <definedName name="DBFsource98aa8cc9d51a47f285383d9ba114f5ed" hidden="1">'3'!$B$2</definedName>
-    <definedName name="DBFsourced7749c24342e4010ba50d1218bb214cc" hidden="1">'3'!#REF!</definedName>
     <definedName name="DBFsourcef456e31645e64ce48a60365aaba7b46a" hidden="1">'3'!$B$15</definedName>
     <definedName name="DBFsourcef5a330494f3e4e92aa635ef5834d3fcd" hidden="1">'2'!$A$6</definedName>
     <definedName name="DBFtarget0d6e4daa4bc1480498245f08c4eb094b" hidden="1">'1'!$E$1:$I$9</definedName>
-    <definedName name="DBFtarget663f4cc231bd4c42bd757fd9e6d2c563" hidden="1">'3'!$A$20:$I$66</definedName>
-    <definedName name="DBFtarget98aa8cc9d51a47f285383d9ba114f5ed" hidden="1">'3'!$A$3:$H$13</definedName>
+    <definedName name="DBFtarget663f4cc231bd4c42bd757fd9e6d2c563" hidden="1">'3'!$A$20:$I$63</definedName>
+    <definedName name="DBFtarget98aa8cc9d51a47f285383d9ba114f5ed" hidden="1">'3'!$A$3:$H$12</definedName>
     <definedName name="DBFtargetf456e31645e64ce48a60365aaba7b46a" hidden="1">'3'!$A$16:$H$17</definedName>
-    <definedName name="DBFtargetf5a330494f3e4e92aa635ef5834d3fcd" hidden="1">'2'!$F$1:$J$6</definedName>
+    <definedName name="DBFtargetf5a330494f3e4e92aa635ef5834d3fcd" hidden="1">'2'!$F$1:$U$17</definedName>
     <definedName name="ExterneDaten_1" localSheetId="1" hidden="1">'1'!$E$1:$I$9</definedName>
-    <definedName name="ExterneDaten_1" localSheetId="3" hidden="1">'3'!$A$3:$H$13</definedName>
-    <definedName name="ExterneDaten_2" localSheetId="3" hidden="1">'3'!$A$20:$H$66</definedName>
+    <definedName name="ExterneDaten_1" localSheetId="3" hidden="1">'3'!$A$3:$H$12</definedName>
+    <definedName name="ExterneDaten_2" localSheetId="3" hidden="1">'3'!$A$20:$H$63</definedName>
     <definedName name="ExterneDaten_3" localSheetId="3" hidden="1">'3'!$A$16:$H$17</definedName>
     <definedName name="testUnderlyingName">Tabelle_ExterneDaten_2[#All]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="78" r:id="rId5"/>
+    <pivotCache cacheId="42" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -61,7 +60,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" keepAlive="1" name="LENOVO-PC pubs sales" type="5" refreshedVersion="8">
-    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL Server Native Client 11.0;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="select * from jobs where job_desc like 'p%'"/>
+    <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL Server Native Client 11.0;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="select * from jobs where job_desc like '%'"/>
   </connection>
   <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" keepAlive="1" name="listobject0" type="5" refreshedVersion="8" saveData="1">
     <dbPr connection="Provider=SQLOLEDB.1;Persist Security Info=True;Extended Properties=&quot;driver=SQL Server Native Client 11.0;Server=Lenovo-PC;Trusted_Connection=Yes;Database=pubs&quot;;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=32767;Workstation ID=LENOVO-PC;Use Encryption for Data=False;Tag with column collation when possible=False" command="select * from publishers where  country like '%'"/>
@@ -79,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="232">
   <si>
     <t>France</t>
   </si>
@@ -324,9 +323,6 @@
     <t>F-C16315M</t>
   </si>
   <si>
-    <t>PMA42628M</t>
-  </si>
-  <si>
     <t>Paolo</t>
   </si>
   <si>
@@ -729,30 +725,12 @@
     <t>Ariadne</t>
   </si>
   <si>
-    <t>DZT39435M</t>
-  </si>
-  <si>
-    <t>iouiz</t>
-  </si>
-  <si>
-    <t>iuziuz</t>
-  </si>
-  <si>
     <t>DBSetQuery function, ListObject</t>
   </si>
   <si>
     <t>München</t>
   </si>
   <si>
-    <t>DGT39435M</t>
-  </si>
-  <si>
-    <t>ghjjh</t>
-  </si>
-  <si>
-    <t>ghjghj</t>
-  </si>
-  <si>
     <t>DBSetQuery functions, multiple ListObjects, different referring to target (single header cell, whole header, range name), multiple underlying names</t>
   </si>
   <si>
@@ -760,6 +738,42 @@
   </si>
   <si>
     <t>FullName</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Acquisitions Manager</t>
+  </si>
+  <si>
+    <t>Business Operations Manager</t>
+  </si>
+  <si>
+    <t>Chief Executive Officer</t>
+  </si>
+  <si>
+    <t>Chief Financial Officier</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>Editor</t>
+  </si>
+  <si>
+    <t>Managing Editor</t>
+  </si>
+  <si>
+    <t>Marketing Manager</t>
+  </si>
+  <si>
+    <t>New Hire - Job not specified</t>
+  </si>
+  <si>
+    <t>Operations Manager</t>
+  </si>
+  <si>
+    <t>Sales Representative</t>
   </si>
 </sst>
 </file>
@@ -841,7 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -856,28 +870,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="16">
     <dxf>
       <numFmt numFmtId="20" formatCode="dd/mmm/yy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="20" formatCode="dd/mmm/yy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -895,63 +902,7 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="20" formatCode="dd/mmm/yy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1044,57 +995,68 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="roland kapl" refreshedDate="45157.47819710648" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="3" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="roland kapl" refreshedDate="45561.981961921294" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="14" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="job_id" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="14" count="14">
+        <n v="1"/>
+        <n v="2"/>
+        <n v="3"/>
+        <n v="4"/>
         <n v="5"/>
+        <n v="6"/>
+        <n v="7"/>
         <n v="8"/>
+        <n v="9"/>
         <n v="10"/>
-        <n v="13" u="1"/>
-        <n v="14" u="1"/>
-        <n v="2" u="1"/>
-        <n v="6" u="1"/>
-        <n v="7" u="1"/>
-        <n v="1" u="1"/>
-        <n v="3" u="1"/>
-        <n v="9" u="1"/>
-        <n v="11" u="1"/>
-        <n v="4" u="1"/>
-        <n v="12" u="1"/>
+        <n v="11"/>
+        <n v="12"/>
+        <n v="13"/>
+        <n v="14"/>
       </sharedItems>
     </cacheField>
     <cacheField name="job_desc" numFmtId="0">
       <sharedItems count="14">
+        <s v="New Hire - Job not specified"/>
+        <s v="Chief Executive Officer"/>
+        <s v="Business Operations Manager"/>
+        <s v="Chief Financial Officier"/>
         <s v="Publisher"/>
+        <s v="Managing Editor"/>
+        <s v="Marketing Manager"/>
         <s v="Public Relations Manager"/>
+        <s v="Acquisitions Manager"/>
         <s v="Productions Manager"/>
-        <s v="Chief Financial Officier" u="1"/>
-        <s v="Acquisitions Manager" u="1"/>
-        <s v="Managing Editor" u="1"/>
-        <s v="Business Operations Manager" u="1"/>
-        <s v="Operations Manager" u="1"/>
-        <s v="Editor" u="1"/>
-        <s v="Sales Representative" u="1"/>
-        <s v="New Hire - Job not specified" u="1"/>
-        <s v="Marketing Manager" u="1"/>
-        <s v="Designer" u="1"/>
-        <s v="Chief Executive Officer" u="1"/>
+        <s v="Operations Manager"/>
+        <s v="Editor"/>
+        <s v="Sales Representative"/>
+        <s v="Designer"/>
       </sharedItems>
     </cacheField>
     <cacheField name="min_lvl" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="75" maxValue="150" count="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="200" count="9">
+        <n v="10"/>
+        <n v="200"/>
+        <n v="175"/>
         <n v="150"/>
+        <n v="140"/>
+        <n v="120"/>
         <n v="100"/>
         <n v="75"/>
+        <n v="25"/>
       </sharedItems>
     </cacheField>
     <cacheField name="max_lvl" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="165" maxValue="250" count="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="10" maxValue="250" count="8">
+        <n v="10"/>
         <n v="250"/>
+        <n v="225"/>
+        <n v="200"/>
         <n v="175"/>
         <n v="165"/>
+        <n v="150"/>
+        <n v="100"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1107,7 +1069,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="3">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="14">
   <r>
     <x v="0"/>
     <x v="0"/>
@@ -1126,48 +1088,114 @@
     <x v="2"/>
     <x v="2"/>
   </r>
+  <r>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="5"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="6"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="8"/>
+    <x v="8"/>
+    <x v="7"/>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="9"/>
+    <x v="9"/>
+    <x v="7"/>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="10"/>
+    <x v="10"/>
+    <x v="7"/>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="11"/>
+    <x v="11"/>
+    <x v="8"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="12"/>
+    <x v="12"/>
+    <x v="8"/>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="13"/>
+    <x v="13"/>
+    <x v="8"/>
+    <x v="7"/>
+  </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="78" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="F1:J6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="F1:U17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
       <items count="15">
-        <item m="1" x="8"/>
-        <item m="1" x="5"/>
-        <item m="1" x="9"/>
-        <item m="1" x="12"/>
         <item x="0"/>
-        <item m="1" x="6"/>
-        <item m="1" x="7"/>
         <item x="1"/>
-        <item m="1" x="10"/>
         <item x="2"/>
-        <item m="1" x="11"/>
-        <item m="1" x="13"/>
-        <item m="1" x="3"/>
-        <item m="1" x="4"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="15">
-        <item m="1" x="4"/>
-        <item m="1" x="6"/>
-        <item m="1" x="13"/>
-        <item m="1" x="3"/>
-        <item m="1" x="12"/>
-        <item m="1" x="8"/>
-        <item m="1" x="5"/>
-        <item m="1" x="11"/>
-        <item m="1" x="10"/>
-        <item m="1" x="7"/>
+        <item x="8"/>
         <item x="2"/>
         <item x="1"/>
+        <item x="3"/>
+        <item x="13"/>
+        <item x="11"/>
+        <item x="5"/>
+        <item x="6"/>
         <item x="0"/>
-        <item m="1" x="9"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="12"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1177,7 +1205,37 @@
   <rowFields count="1">
     <field x="1"/>
   </rowFields>
-  <rowItems count="4">
+  <rowItems count="15">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
     <i>
       <x v="10"/>
     </i>
@@ -1187,6 +1245,9 @@
     <i>
       <x v="12"/>
     </i>
+    <i>
+      <x v="13"/>
+    </i>
     <i t="grand">
       <x/>
     </i>
@@ -1194,15 +1255,48 @@
   <colFields count="1">
     <field x="0"/>
   </colFields>
-  <colItems count="4">
+  <colItems count="15">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
     <i>
       <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
     </i>
     <i>
       <x v="7"/>
     </i>
     <i>
+      <x v="8"/>
+    </i>
+    <i>
       <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
     </i>
     <i t="grand">
       <x/>
@@ -1239,16 +1333,16 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExterneDaten_1" backgroundRefresh="0" adjustColumnWidth="0" connectionId="3" xr16:uid="{AA89DD0C-7585-4C80-B75D-DDCC1C58B3A4}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="18">
+  <queryTableRefresh nextId="9">
     <queryTableFields count="8">
-      <queryTableField id="2" name="emp_id" tableColumnId="3"/>
-      <queryTableField id="3" name="fname" tableColumnId="4"/>
-      <queryTableField id="4" name="minit" tableColumnId="5"/>
-      <queryTableField id="5" name="lname" tableColumnId="6"/>
-      <queryTableField id="6" name="job_id" tableColumnId="7"/>
-      <queryTableField id="7" name="job_lvl" tableColumnId="8"/>
-      <queryTableField id="8" name="pub_id" tableColumnId="9"/>
-      <queryTableField id="9" name="hire_date" tableColumnId="10"/>
+      <queryTableField id="1" name="emp_id" tableColumnId="1"/>
+      <queryTableField id="2" name="fname" tableColumnId="2"/>
+      <queryTableField id="3" name="minit" tableColumnId="3"/>
+      <queryTableField id="4" name="lname" tableColumnId="4"/>
+      <queryTableField id="5" name="job_id" tableColumnId="5"/>
+      <queryTableField id="6" name="job_lvl" tableColumnId="6"/>
+      <queryTableField id="7" name="pub_id" tableColumnId="7"/>
+      <queryTableField id="8" name="hire_date" tableColumnId="8"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -1293,46 +1387,46 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Abfrage1" displayName="Abfrage1" ref="E1:I9" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="E1:I9" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="pub_id" queryTableFieldId="1" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="pub_name" queryTableFieldId="2" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="city" queryTableFieldId="3" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="state" queryTableFieldId="4" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="country" queryTableFieldId="5" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="1" name="pub_id" queryTableFieldId="1" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="2" name="pub_name" queryTableFieldId="2" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="3" name="city" queryTableFieldId="3" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" uniqueName="4" name="state" queryTableFieldId="4" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" uniqueName="5" name="country" queryTableFieldId="5" dataDxfId="11"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D077F9AA-5529-4224-9F94-DA11CB704393}" name="Tabelle_ExterneDaten_1" displayName="Tabelle_ExterneDaten_1" ref="A3:H13" tableType="queryTable" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
-  <autoFilter ref="A3:H13" xr:uid="{D077F9AA-5529-4224-9F94-DA11CB704393}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D077F9AA-5529-4224-9F94-DA11CB704393}" name="Tabelle_ExterneDaten_1" displayName="Tabelle_ExterneDaten_1" ref="A3:H12" tableType="queryTable" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="A3:H12" xr:uid="{D077F9AA-5529-4224-9F94-DA11CB704393}"/>
   <tableColumns count="8">
-    <tableColumn id="3" xr3:uid="{7211A85E-BEFA-46CF-920D-FBA1477F0FA8}" uniqueName="3" name="emp_id" queryTableFieldId="2" dataDxfId="17" dataCellStyle="Standard 2"/>
-    <tableColumn id="4" xr3:uid="{D413397E-DEB9-4ED0-9AAF-9302A5A25CB3}" uniqueName="4" name="fname" queryTableFieldId="3" dataDxfId="16" dataCellStyle="Standard 2"/>
-    <tableColumn id="5" xr3:uid="{042493AF-922D-4339-BDD0-DFF6E133B8ED}" uniqueName="5" name="minit" queryTableFieldId="4" dataDxfId="15" dataCellStyle="Standard 2"/>
-    <tableColumn id="6" xr3:uid="{A7E6ADB2-09B5-4F3C-90BE-2EF2B0147380}" uniqueName="6" name="lname" queryTableFieldId="5" dataDxfId="14" dataCellStyle="Standard 2"/>
-    <tableColumn id="7" xr3:uid="{FCA7BDA4-4142-4EF6-9DB3-B865E698544E}" uniqueName="7" name="job_id" queryTableFieldId="6" dataDxfId="13" dataCellStyle="Standard 2"/>
-    <tableColumn id="8" xr3:uid="{763B5A20-D2CC-4849-BA15-1432EC39EAD7}" uniqueName="8" name="job_lvl" queryTableFieldId="7" dataDxfId="12" dataCellStyle="Standard 2"/>
-    <tableColumn id="9" xr3:uid="{BACCA8F3-E7B8-4792-BAA7-761791710302}" uniqueName="9" name="pub_id" queryTableFieldId="8" dataDxfId="11" dataCellStyle="Standard 2"/>
-    <tableColumn id="10" xr3:uid="{FDEC2839-8AE6-4527-917D-04864CC4CD63}" uniqueName="10" name="hire_date" queryTableFieldId="9" dataDxfId="10" dataCellStyle="Standard 2"/>
+    <tableColumn id="1" xr3:uid="{9063AED2-1F8C-46CD-89C5-376E796406CC}" uniqueName="1" name="emp_id" queryTableFieldId="1" dataCellStyle="Standard 2"/>
+    <tableColumn id="2" xr3:uid="{BFD12F9E-21D3-4ACF-A6AA-163A2135D10C}" uniqueName="2" name="fname" queryTableFieldId="2" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{9F787658-29C9-47E0-B49F-AED307836C28}" uniqueName="3" name="minit" queryTableFieldId="3" dataCellStyle="Standard 2"/>
+    <tableColumn id="4" xr3:uid="{AEC8B88F-E9A9-41CA-9453-34AB937E6BFF}" uniqueName="4" name="lname" queryTableFieldId="4" dataCellStyle="Standard 2"/>
+    <tableColumn id="5" xr3:uid="{A2175D36-9AE8-43F1-98C7-64AA1F79BE68}" uniqueName="5" name="job_id" queryTableFieldId="5" dataCellStyle="Standard 2"/>
+    <tableColumn id="6" xr3:uid="{702F8EDC-BF8F-4491-9C31-BB133E5E74D7}" uniqueName="6" name="job_lvl" queryTableFieldId="6" dataCellStyle="Standard 2"/>
+    <tableColumn id="7" xr3:uid="{12B32319-EC8F-4B98-A5B9-6546CC822FC6}" uniqueName="7" name="pub_id" queryTableFieldId="7" dataCellStyle="Standard 2"/>
+    <tableColumn id="8" xr3:uid="{ABC8CEC1-C714-4DDD-80F1-16BF0927F555}" uniqueName="8" name="hire_date" queryTableFieldId="8" dataDxfId="0" dataCellStyle="Standard 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18660A67-20A6-401F-896C-A253966CD939}" name="Tabelle_ExterneDaten_2" displayName="Tabelle_ExterneDaten_2" ref="A20:I66" tableType="queryTable" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
-  <autoFilter ref="A20:I66" xr:uid="{18660A67-20A6-401F-896C-A253966CD939}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{18660A67-20A6-401F-896C-A253966CD939}" name="Tabelle_ExterneDaten_2" displayName="Tabelle_ExterneDaten_2" ref="A20:I63" tableType="queryTable" totalsRowShown="0" headerRowCellStyle="Standard 2" dataCellStyle="Standard 2">
+  <autoFilter ref="A20:I63" xr:uid="{18660A67-20A6-401F-896C-A253966CD939}"/>
   <tableColumns count="9">
-    <tableColumn id="3" xr3:uid="{36756E84-6476-4520-A091-157D1B54BA4A}" uniqueName="3" name="emp_id" queryTableFieldId="2" dataDxfId="9" dataCellStyle="Standard 2"/>
-    <tableColumn id="4" xr3:uid="{1D6AA48D-3BA9-42F7-AE89-F4153E79CCE6}" uniqueName="4" name="fname" queryTableFieldId="3" dataDxfId="8" dataCellStyle="Standard 2"/>
-    <tableColumn id="5" xr3:uid="{6A942B7A-BE3E-4728-8B98-2AF44675A55A}" uniqueName="5" name="minit" queryTableFieldId="4" dataDxfId="7" dataCellStyle="Standard 2"/>
-    <tableColumn id="6" xr3:uid="{61596B93-AB0B-4B84-B06B-67963353BC71}" uniqueName="6" name="lname" queryTableFieldId="5" dataDxfId="6" dataCellStyle="Standard 2"/>
-    <tableColumn id="7" xr3:uid="{DA148D9C-ED55-4A55-A735-D448C6D4B958}" uniqueName="7" name="job_id" queryTableFieldId="6" dataDxfId="5" dataCellStyle="Standard 2"/>
-    <tableColumn id="8" xr3:uid="{48381964-EB05-4B0E-97BB-10967E8923A0}" uniqueName="8" name="job_lvl" queryTableFieldId="7" dataDxfId="4" dataCellStyle="Standard 2"/>
-    <tableColumn id="9" xr3:uid="{12E7DC44-9215-45EF-ACA3-923FE7BA6813}" uniqueName="9" name="pub_id" queryTableFieldId="8" dataDxfId="3" dataCellStyle="Standard 2"/>
+    <tableColumn id="3" xr3:uid="{36756E84-6476-4520-A091-157D1B54BA4A}" uniqueName="3" name="emp_id" queryTableFieldId="2" dataDxfId="10" dataCellStyle="Standard 2"/>
+    <tableColumn id="4" xr3:uid="{1D6AA48D-3BA9-42F7-AE89-F4153E79CCE6}" uniqueName="4" name="fname" queryTableFieldId="3" dataDxfId="9" dataCellStyle="Standard 2"/>
+    <tableColumn id="5" xr3:uid="{6A942B7A-BE3E-4728-8B98-2AF44675A55A}" uniqueName="5" name="minit" queryTableFieldId="4" dataDxfId="8" dataCellStyle="Standard 2"/>
+    <tableColumn id="6" xr3:uid="{61596B93-AB0B-4B84-B06B-67963353BC71}" uniqueName="6" name="lname" queryTableFieldId="5" dataDxfId="7" dataCellStyle="Standard 2"/>
+    <tableColumn id="7" xr3:uid="{DA148D9C-ED55-4A55-A735-D448C6D4B958}" uniqueName="7" name="job_id" queryTableFieldId="6" dataDxfId="6" dataCellStyle="Standard 2"/>
+    <tableColumn id="8" xr3:uid="{48381964-EB05-4B0E-97BB-10967E8923A0}" uniqueName="8" name="job_lvl" queryTableFieldId="7" dataDxfId="5" dataCellStyle="Standard 2"/>
+    <tableColumn id="9" xr3:uid="{12E7DC44-9215-45EF-ACA3-923FE7BA6813}" uniqueName="9" name="pub_id" queryTableFieldId="8" dataDxfId="4" dataCellStyle="Standard 2"/>
     <tableColumn id="10" xr3:uid="{D8BCD53C-8895-4795-AAD6-51DC52FEE94F}" uniqueName="10" name="hire_date" queryTableFieldId="9" dataDxfId="2" dataCellStyle="Standard 2"/>
-    <tableColumn id="11" xr3:uid="{440132AD-A5A8-4107-A616-988EE8E2286F}" uniqueName="11" name="FullName" queryTableFieldId="10" dataDxfId="1" dataCellStyle="Standard 2">
+    <tableColumn id="11" xr3:uid="{440132AD-A5A8-4107-A616-988EE8E2286F}" uniqueName="11" name="FullName" queryTableFieldId="10" dataDxfId="3" dataCellStyle="Standard 2">
       <calculatedColumnFormula>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1351,16 +1445,16 @@
     <tableColumn id="31" xr3:uid="{CDE367BA-72B0-4353-AA2D-14B714B22939}" uniqueName="31" name="job_id" queryTableFieldId="5" dataCellStyle="Standard 2"/>
     <tableColumn id="32" xr3:uid="{52435267-4833-407F-BEB4-7BD9095F47E5}" uniqueName="32" name="job_lvl" queryTableFieldId="6" dataCellStyle="Standard 2"/>
     <tableColumn id="33" xr3:uid="{3DDAEEAE-5D2C-4B8C-8066-B44397CD4D62}" uniqueName="33" name="pub_id" queryTableFieldId="7" dataCellStyle="Standard 2"/>
-    <tableColumn id="34" xr3:uid="{E65C2FC8-60EF-48E3-8441-EBB1B9A71822}" uniqueName="34" name="hire_date" queryTableFieldId="8" dataDxfId="0" dataCellStyle="Standard 2"/>
+    <tableColumn id="34" xr3:uid="{E65C2FC8-60EF-48E3-8441-EBB1B9A71822}" uniqueName="34" name="hire_date" queryTableFieldId="8" dataDxfId="1" dataCellStyle="Standard 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1398,7 +1492,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1504,7 +1598,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1646,7 +1740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1657,7 +1751,7 @@
   <sheetPr codeName="ConnSetting"/>
   <dimension ref="A1:K1233"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -2016,12 +2110,12 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="149.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -2031,7 +2125,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="E1" t="s">
         <v>58</v>
@@ -2069,7 +2163,7 @@
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>_xll.DBSetQuery("select * from publishers where  country like "&amp;_xll.DBString(A4),activeConnString,Abfrage1[#All])</f>
-        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False, ): select * from publishers where  country like '%'</v>
+        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False), : select * from publishers where  country like '%'</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
@@ -2149,40 +2243,41 @@
         <v>10</v>
       </c>
       <c r="G7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="I7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E8" t="s">
+      <c r="E8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="15" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E9" t="s">
+      <c r="E9" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
+      <c r="H9" s="15"/>
+      <c r="I9" s="15" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2197,23 +2292,21 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="20" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="20" width="4" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>51</v>
       </c>
@@ -2224,87 +2317,448 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F2" s="8" t="s">
         <v>49</v>
       </c>
       <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
         <v>5</v>
       </c>
-      <c r="H2">
+      <c r="L2">
+        <v>6</v>
+      </c>
+      <c r="M2">
+        <v>7</v>
+      </c>
+      <c r="N2">
         <v>8</v>
       </c>
-      <c r="I2">
+      <c r="O2">
+        <v>9</v>
+      </c>
+      <c r="P2">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="Q2">
+        <v>11</v>
+      </c>
+      <c r="R2">
+        <v>12</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2">
+        <v>14</v>
+      </c>
+      <c r="U2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="F3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12">
-        <v>165</v>
-      </c>
-      <c r="J3" s="12">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>221</v>
+      </c>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15">
+        <v>175</v>
+      </c>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12">
-        <v>175</v>
-      </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>60</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15">
+        <v>225</v>
+      </c>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
+      <c r="T4" s="15"/>
+      <c r="U4" s="15">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="10"/>
       <c r="F5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="G5" s="12">
+        <v>223</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15">
         <v>250</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12">
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15">
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>_xll.DBSetQuery("select * from jobs where job_desc like "&amp;_xll.DBString(A5,"%"),activeConnString,F1)</f>
-        <v>Env:MSSQL, (last result:)Set OLEDB; PivotTable to (bgQuery= False): select * from jobs where job_desc like 'p%'</v>
+        <v>Env:MSSQL, (last result:)Set OLEDB; PivotTable to (bgQuery= False): select * from jobs where job_desc like '%'</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15">
+        <v>250</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F7" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15">
+        <v>100</v>
+      </c>
+      <c r="U7" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F8" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15"/>
+      <c r="R8" s="15">
+        <v>100</v>
+      </c>
+      <c r="S8" s="15"/>
+      <c r="T8" s="15"/>
+      <c r="U8" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F9" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15">
+        <v>225</v>
+      </c>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F10" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15">
+        <v>200</v>
+      </c>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
+      <c r="P10" s="15"/>
+      <c r="Q10" s="15"/>
+      <c r="R10" s="15"/>
+      <c r="S10" s="15"/>
+      <c r="T10" s="15"/>
+      <c r="U10" s="15">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F11" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="G11" s="15">
+        <v>10</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F12" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15">
+        <v>150</v>
+      </c>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15">
+        <v>165</v>
+      </c>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15"/>
+      <c r="S13" s="15"/>
+      <c r="T13" s="15"/>
+      <c r="U13" s="15">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F14" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="15">
+        <v>175</v>
+      </c>
+      <c r="O14" s="15"/>
+      <c r="P14" s="15"/>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15"/>
+      <c r="S14" s="15"/>
+      <c r="T14" s="15"/>
+      <c r="U14" s="15">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F15" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15">
+        <v>250</v>
+      </c>
+      <c r="L15" s="15"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="15"/>
+      <c r="O15" s="15"/>
+      <c r="P15" s="15"/>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15"/>
+      <c r="S15" s="15"/>
+      <c r="T15" s="15"/>
+      <c r="U15" s="15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="F16" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15">
+        <v>100</v>
+      </c>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="6:21" x14ac:dyDescent="0.2">
+      <c r="F17" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G17" s="15">
+        <v>10</v>
+      </c>
+      <c r="H17" s="15">
         <v>250</v>
       </c>
-      <c r="H6" s="12">
+      <c r="I17" s="15">
+        <v>225</v>
+      </c>
+      <c r="J17" s="15">
+        <v>250</v>
+      </c>
+      <c r="K17" s="15">
+        <v>250</v>
+      </c>
+      <c r="L17" s="15">
+        <v>225</v>
+      </c>
+      <c r="M17" s="15">
+        <v>200</v>
+      </c>
+      <c r="N17" s="15">
         <v>175</v>
       </c>
-      <c r="I6" s="12">
+      <c r="O17" s="15">
+        <v>175</v>
+      </c>
+      <c r="P17" s="15">
         <v>165</v>
       </c>
-      <c r="J6" s="12">
-        <v>590</v>
+      <c r="Q17" s="15">
+        <v>150</v>
+      </c>
+      <c r="R17" s="15">
+        <v>100</v>
+      </c>
+      <c r="S17" s="15">
+        <v>100</v>
+      </c>
+      <c r="T17" s="15">
+        <v>100</v>
+      </c>
+      <c r="U17" s="15">
+        <v>2375</v>
       </c>
     </row>
   </sheetData>
@@ -2315,9 +2769,9 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -2395,336 +2849,313 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>60</v>
       </c>
       <c r="B2" s="11" t="str">
         <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A2,"%"),"",Tabelle_ExterneDaten_1[[#Headers],[emp_id]])</f>
-        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False, ): select * from employee where fname like 'p%'</v>
+        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False), : select * from employee where fname like 'p%'</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="11">
         <v>10</v>
       </c>
       <c r="F4" s="11">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="13">
         <v>39017.034039351849</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D5" s="13" t="s">
+      <c r="A5" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="13">
-        <v>13</v>
-      </c>
-      <c r="F5" s="13">
-        <v>35</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="B5" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="11">
+        <v>14</v>
+      </c>
+      <c r="F5" s="11">
+        <v>89</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="13">
+        <v>33231</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="E6" s="11">
+        <v>6</v>
+      </c>
+      <c r="F6" s="11">
+        <v>215</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="13">
+        <v>32823</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E7" s="11">
+        <v>10</v>
+      </c>
+      <c r="F7" s="11">
+        <v>77</v>
+      </c>
+      <c r="G7" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="15">
-        <v>33843</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="B6" s="13" t="s">
+      <c r="H7" s="13">
+        <v>33741</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="11">
+        <v>5</v>
+      </c>
+      <c r="F8" s="11">
+        <v>159</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="13">
+        <v>34200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="E9" s="11">
+        <v>7</v>
+      </c>
+      <c r="F9" s="11">
+        <v>195</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="13">
+        <v>34098</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E10" s="11">
+        <v>10</v>
+      </c>
+      <c r="F10" s="11">
+        <v>80</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="13">
+        <v>34302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>157</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="E11" s="11">
+        <v>11</v>
+      </c>
+      <c r="F11" s="11">
+        <v>150</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="13">
+        <v>32721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="13">
-        <v>14</v>
-      </c>
-      <c r="F6" s="13">
-        <v>89</v>
-      </c>
-      <c r="G6" s="13" t="s">
+      <c r="D12" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="11">
+        <v>8</v>
+      </c>
+      <c r="F12" s="11">
+        <v>125</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="15">
-        <v>33231</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" s="13">
-        <v>6</v>
-      </c>
-      <c r="F7" s="13">
-        <v>215</v>
-      </c>
-      <c r="G7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="15">
-        <v>32823</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>108</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E8" s="13">
-        <v>10</v>
-      </c>
-      <c r="F8" s="13">
-        <v>75</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="15">
-        <v>33741</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E9" s="13">
-        <v>5</v>
-      </c>
-      <c r="F9" s="13">
-        <v>159</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H9" s="15">
-        <v>34200</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E10" s="13">
-        <v>7</v>
-      </c>
-      <c r="F10" s="13">
-        <v>195</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="15">
-        <v>34098</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E11" s="13">
-        <v>10</v>
-      </c>
-      <c r="F11" s="13">
-        <v>80</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="15">
-        <v>34302</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>156</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E12" s="13">
-        <v>11</v>
-      </c>
-      <c r="F12" s="13">
-        <v>150</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="15">
-        <v>32721</v>
+      <c r="H12" s="13">
+        <v>34353</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>178</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="E13" s="13">
-        <v>8</v>
-      </c>
-      <c r="F13" s="13">
-        <v>125</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H13" s="15">
-        <v>34353</v>
-      </c>
+      <c r="H13" s="13"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
-        <v>225</v>
+      <c r="A15" s="12" t="s">
+        <v>218</v>
       </c>
       <c r="B15" s="11" t="str">
         <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A15,"%"),"",Tabelle_ExterneDaten_15[#Headers])</f>
-        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False, ): select * from employee where fname like 'f%'</v>
+        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False), : select * from employee where fname like 'f%'</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F16" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G16" s="13" t="s">
+      <c r="G16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="H16" s="11" t="s">
         <v>71</v>
       </c>
     </row>
@@ -2747,1414 +3178,1326 @@
       <c r="G17" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="15">
+      <c r="H17" s="13">
         <v>33180</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-    </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="12"/>
       <c r="B19" s="11" t="str">
         <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A19,"%"),"",testUnderlyingName)</f>
-        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False, ): select * from employee where fname like '%'</v>
+        <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False), : select * from employee where fname like '%'</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F20" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="I20" s="16" t="s">
-        <v>226</v>
+      <c r="I20" s="14" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>62</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="11">
         <v>10</v>
       </c>
       <c r="F21" s="11">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H21" s="15">
+      <c r="H21" s="13">
         <v>39017.034039351849</v>
       </c>
-      <c r="I21" s="13" t="str">
+      <c r="I21" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Paolo A Accorti</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B22" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E22" s="13">
-        <v>13</v>
-      </c>
-      <c r="F22" s="13">
-        <v>35</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22" s="15">
-        <v>33843</v>
-      </c>
-      <c r="I22" s="13" t="str">
-        <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
-        <v>Paolo M Accorti</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="B22" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="C22" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="D22" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="D23" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" s="13">
+      <c r="E22" s="11">
         <v>14</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F22" s="11">
         <v>89</v>
       </c>
-      <c r="G23" s="13" t="s">
+      <c r="G22" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H23" s="15">
+      <c r="H22" s="13">
         <v>33231</v>
       </c>
-      <c r="I23" s="13" t="str">
+      <c r="I22" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Pedro S Afonso</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="C23" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="D23" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" s="13">
+      <c r="E23" s="11">
         <v>6</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F23" s="11">
         <v>140</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G23" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H24" s="15">
+      <c r="H23" s="13">
         <v>33129</v>
       </c>
-      <c r="I24" s="13" t="str">
+      <c r="I23" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Victoria P Ashworth</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13" t="s">
+      <c r="D24" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E24" s="11">
         <v>5</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F24" s="11">
         <v>160</v>
       </c>
-      <c r="G25" s="13" t="s">
+      <c r="G24" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H24" s="13">
         <v>32772</v>
       </c>
-      <c r="I25" s="13" t="str">
+      <c r="I24" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Helen  Bennett</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="C25" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D25" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E26" s="13">
+      <c r="E25" s="11">
         <v>7</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F25" s="11">
         <v>120</v>
       </c>
-      <c r="G26" s="13" t="s">
+      <c r="G25" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H25" s="13">
         <v>33282</v>
       </c>
-      <c r="I26" s="13" t="str">
+      <c r="I25" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Lesley a Brown</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B26" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13" t="s">
+      <c r="D26" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E26" s="11">
         <v>4</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F26" s="11">
         <v>227</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G26" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H26" s="13">
         <v>33180</v>
       </c>
-      <c r="I27" s="13" t="str">
+      <c r="I26" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Francisco  Chang</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="C27" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="D27" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D28" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E28" s="13">
+      <c r="E27" s="11">
         <v>6</v>
       </c>
-      <c r="F28" s="13">
+      <c r="F27" s="11">
         <v>215</v>
       </c>
-      <c r="G28" s="13" t="s">
+      <c r="G27" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H27" s="13">
         <v>32823</v>
       </c>
-      <c r="I28" s="13" t="str">
+      <c r="I27" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Philip T Cramer</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>214</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="B29" s="13" t="s">
-        <v>215</v>
-      </c>
-      <c r="C29" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="D29" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="13">
+      <c r="E28" s="11">
         <v>10</v>
       </c>
-      <c r="F29" s="13">
+      <c r="F28" s="11">
         <v>87</v>
       </c>
-      <c r="G29" s="13" t="s">
+      <c r="G28" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H28" s="13">
         <v>33537</v>
       </c>
-      <c r="I29" s="13" t="str">
+      <c r="I28" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Ariadne a Cruz</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="C29" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="13">
+      <c r="E29" s="11">
         <v>3</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F29" s="11">
         <v>200</v>
       </c>
-      <c r="G30" s="13" t="s">
+      <c r="G29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="15">
+      <c r="H29" s="13">
         <v>33435</v>
       </c>
-      <c r="I30" s="13" t="str">
+      <c r="I29" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Ann M Devon</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B30" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="C30" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="D30" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="E31" s="13">
+      <c r="E30" s="11">
         <v>10</v>
       </c>
-      <c r="F31" s="13">
-        <v>75</v>
-      </c>
-      <c r="G31" s="13" t="s">
+      <c r="F30" s="11">
+        <v>77</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H31" s="15">
+      <c r="H30" s="13">
         <v>33741</v>
       </c>
-      <c r="I31" s="13" t="str">
+      <c r="I30" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Peter H Franken</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="E32" s="13">
-        <v>7</v>
-      </c>
-      <c r="F32" s="13">
-        <v>170</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32" s="15">
-        <v>40001</v>
-      </c>
-      <c r="I32" s="13" t="str">
-        <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
-        <v>ghjjh  ghjghj</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B31" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="C31" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="D31" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="D33" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="E33" s="13">
+      <c r="E31" s="11">
         <v>5</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F31" s="11">
         <v>159</v>
       </c>
-      <c r="G33" s="13" t="s">
+      <c r="G31" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H31" s="13">
         <v>34200</v>
       </c>
-      <c r="I33" s="13" t="str">
+      <c r="I31" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Paul X Henriot</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B32" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="C32" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="D32" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D34" s="13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E34" s="13">
+      <c r="E32" s="11">
         <v>5</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F32" s="11">
         <v>211</v>
       </c>
-      <c r="G34" s="13" t="s">
+      <c r="G32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H34" s="15">
+      <c r="H32" s="13">
         <v>32619</v>
       </c>
-      <c r="I34" s="13" t="str">
+      <c r="I32" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Carlos F Hernadez</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="C33" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="D33" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="D35" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" s="13">
+      <c r="E33" s="11">
         <v>7</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F33" s="11">
         <v>195</v>
       </c>
-      <c r="G35" s="13" t="s">
+      <c r="G33" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H35" s="15">
+      <c r="H33" s="13">
         <v>34098</v>
       </c>
-      <c r="I35" s="13" t="str">
+      <c r="I33" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Palle D Ibsen</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="B36" s="13" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13" t="s">
-        <v>218</v>
-      </c>
-      <c r="E36" s="13">
-        <v>7</v>
-      </c>
-      <c r="F36" s="13">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="11">
+        <v>9</v>
+      </c>
+      <c r="F34" s="11">
         <v>170</v>
       </c>
-      <c r="G36" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="15">
-        <v>40001</v>
-      </c>
-      <c r="I36" s="13" t="str">
-        <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
-        <v>iouiz  iuziuz</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B37" s="13" t="s">
-        <v>125</v>
-      </c>
-      <c r="C37" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D37" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="E37" s="13">
-        <v>9</v>
-      </c>
-      <c r="F37" s="13">
-        <v>170</v>
-      </c>
-      <c r="G37" s="13" t="s">
+      <c r="G34" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H34" s="13">
         <v>34404</v>
       </c>
-      <c r="I37" s="13" t="str">
+      <c r="I34" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Karla J Jablonski</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="C35" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="C38" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38" s="13">
+      <c r="E35" s="11">
         <v>14</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F35" s="11">
         <v>100</v>
       </c>
-      <c r="G38" s="13" t="s">
+      <c r="G35" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H38" s="15">
+      <c r="H35" s="13">
         <v>33894</v>
       </c>
-      <c r="I38" s="13" t="str">
+      <c r="I35" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Karin F Josephs</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="C36" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="D36" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="13" t="s">
-        <v>134</v>
-      </c>
-      <c r="E39" s="13">
+      <c r="E36" s="11">
         <v>6</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F36" s="11">
         <v>220</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="G36" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H39" s="15">
+      <c r="H36" s="13">
         <v>34455</v>
       </c>
-      <c r="I39" s="13" t="str">
+      <c r="I36" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Matti G Karttunen</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B37" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="C37" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="D37" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="D40" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="13">
+      <c r="E37" s="11">
         <v>10</v>
       </c>
-      <c r="F40" s="13">
+      <c r="F37" s="11">
         <v>80</v>
       </c>
-      <c r="G40" s="13" t="s">
+      <c r="G37" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H37" s="13">
         <v>34302</v>
       </c>
-      <c r="I40" s="13" t="str">
+      <c r="I37" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Pirkko O Koskitalo</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="C38" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="D38" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="D41" s="13" t="s">
-        <v>142</v>
-      </c>
-      <c r="E41" s="13">
+      <c r="E38" s="11">
         <v>5</v>
       </c>
-      <c r="F41" s="13">
+      <c r="F38" s="11">
         <v>172</v>
       </c>
-      <c r="G41" s="13" t="s">
+      <c r="G38" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="15">
+      <c r="H38" s="13">
         <v>33384</v>
       </c>
-      <c r="I41" s="13" t="str">
+      <c r="I38" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Janine Y Labrune</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B39" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="C39" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="D39" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="C42" s="13" t="s">
-        <v>214</v>
-      </c>
-      <c r="D42" s="13" t="s">
-        <v>145</v>
-      </c>
-      <c r="E42" s="13">
+      <c r="E39" s="11">
         <v>7</v>
       </c>
-      <c r="F42" s="13">
+      <c r="F39" s="11">
         <v>135</v>
       </c>
-      <c r="G42" s="13" t="s">
+      <c r="G39" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H42" s="15">
+      <c r="H39" s="13">
         <v>33690</v>
       </c>
-      <c r="I42" s="13" t="str">
+      <c r="I39" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Maria a Larsson</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B40" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="C40" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D40" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="E43" s="13">
+      <c r="E40" s="11">
         <v>12</v>
       </c>
-      <c r="F43" s="13">
-        <v>32</v>
-      </c>
-      <c r="G43" s="13" t="s">
+      <c r="F40" s="11">
+        <v>77</v>
+      </c>
+      <c r="G40" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="15">
+      <c r="H40" s="13">
         <v>32670</v>
       </c>
-      <c r="I43" s="13" t="str">
+      <c r="I40" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Yoshi  Latimer</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="C41" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D41" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="C44" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D44" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="E44" s="13">
+      <c r="E41" s="11">
         <v>5</v>
       </c>
-      <c r="F44" s="13">
+      <c r="F41" s="11">
         <v>175</v>
       </c>
-      <c r="G44" s="13" t="s">
+      <c r="G41" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H44" s="15">
+      <c r="H41" s="13">
         <v>33027</v>
       </c>
-      <c r="I44" s="13" t="str">
+      <c r="I41" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Laurence A Lebihan</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B45" s="13" t="s">
+      <c r="C42" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="D42" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="D45" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="E45" s="13">
+      <c r="E42" s="11">
         <v>14</v>
       </c>
-      <c r="F45" s="13">
-        <v>35</v>
-      </c>
-      <c r="G45" s="13" t="s">
+      <c r="F42" s="11">
+        <v>77</v>
+      </c>
+      <c r="G42" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H45" s="15">
+      <c r="H42" s="13">
         <v>33078</v>
       </c>
-      <c r="I45" s="13" t="str">
+      <c r="I42" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Elizabeth N Lincoln</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="B43" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="C43" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="D43" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="D46" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="E46" s="13">
+      <c r="E43" s="11">
         <v>11</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F43" s="11">
         <v>150</v>
       </c>
-      <c r="G46" s="13" t="s">
+      <c r="G43" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H46" s="15">
+      <c r="H43" s="13">
         <v>32721</v>
       </c>
-      <c r="I46" s="13" t="str">
+      <c r="I43" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Patricia C McKenna</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="B44" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="C44" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D44" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13" t="s">
-        <v>162</v>
-      </c>
-      <c r="E47" s="13">
+      <c r="E44" s="11">
         <v>11</v>
       </c>
-      <c r="F47" s="13">
+      <c r="F44" s="11">
         <v>150</v>
       </c>
-      <c r="G47" s="13" t="s">
+      <c r="G44" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H47" s="15">
+      <c r="H44" s="13">
         <v>33486</v>
       </c>
-      <c r="I47" s="13" t="str">
+      <c r="I44" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Roland  Mendel</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="C45" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="D45" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="D48" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="E48" s="13">
+      <c r="E45" s="11">
         <v>5</v>
       </c>
-      <c r="F48" s="13">
+      <c r="F45" s="11">
         <v>198</v>
       </c>
-      <c r="G48" s="13" t="s">
+      <c r="G45" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H45" s="13">
         <v>34251</v>
       </c>
-      <c r="I48" s="13" t="str">
+      <c r="I45" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Rita B Muller</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B46" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C46" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D46" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E49" s="13">
+      <c r="E46" s="11">
         <v>7</v>
       </c>
-      <c r="F49" s="13">
+      <c r="F46" s="11">
         <v>120</v>
       </c>
-      <c r="G49" s="13" t="s">
+      <c r="G46" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H49" s="15">
+      <c r="H46" s="13">
         <v>34047</v>
       </c>
-      <c r="I49" s="13" t="str">
+      <c r="I46" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Helvetius A Nagy</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>166</v>
+      </c>
+      <c r="B47" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="C47" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D47" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="C50" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="D50" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="E50" s="13">
+      <c r="E47" s="11">
         <v>13</v>
       </c>
-      <c r="F50" s="13">
+      <c r="F47" s="11">
         <v>100</v>
       </c>
-      <c r="G50" s="13" t="s">
+      <c r="G47" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H50" s="15">
+      <c r="H47" s="13">
         <v>32313</v>
       </c>
-      <c r="I50" s="13" t="str">
+      <c r="I47" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Timothy P O'Rourke</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="B48" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="C48" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="D48" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="D51" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="E51" s="13">
+      <c r="E48" s="11">
         <v>5</v>
       </c>
-      <c r="F51" s="13">
+      <c r="F48" s="11">
         <v>150</v>
       </c>
-      <c r="G51" s="13" t="s">
+      <c r="G48" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H51" s="15">
+      <c r="H48" s="13">
         <v>33333</v>
       </c>
-      <c r="I51" s="13" t="str">
+      <c r="I48" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Sven K Ottlieb</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B49" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="C49" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D49" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="C52" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D52" s="13" t="s">
-        <v>176</v>
-      </c>
-      <c r="E52" s="13">
+      <c r="E49" s="11">
         <v>11</v>
       </c>
-      <c r="F52" s="13">
+      <c r="F49" s="11">
         <v>112</v>
       </c>
-      <c r="G52" s="13" t="s">
+      <c r="G49" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H52" s="15">
+      <c r="H49" s="13">
         <v>33945</v>
       </c>
-      <c r="I52" s="13" t="str">
+      <c r="I49" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Miguel A Paolino</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B50" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="C50" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D50" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="C53" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>179</v>
-      </c>
-      <c r="E53" s="13">
+      <c r="E50" s="11">
         <v>8</v>
       </c>
-      <c r="F53" s="13">
+      <c r="F50" s="11">
         <v>125</v>
       </c>
-      <c r="G53" s="13" t="s">
+      <c r="G50" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H53" s="15">
+      <c r="H50" s="13">
         <v>34353</v>
       </c>
-      <c r="I53" s="13" t="str">
+      <c r="I50" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Paula S Parente</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>179</v>
+      </c>
+      <c r="B51" s="11" t="s">
         <v>180</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="C51" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D51" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="E54" s="13">
+      <c r="E51" s="11">
         <v>8</v>
       </c>
-      <c r="F54" s="13">
+      <c r="F51" s="11">
         <v>101</v>
       </c>
-      <c r="G54" s="13" t="s">
+      <c r="G51" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H54" s="15">
+      <c r="H51" s="13">
         <v>32517</v>
       </c>
-      <c r="I54" s="13" t="str">
+      <c r="I51" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Manuel  Pereira</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="11" t="s">
+        <v>182</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D52" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="B55" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C55" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D55" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="E55" s="13">
+      <c r="E52" s="11">
         <v>5</v>
       </c>
-      <c r="F55" s="13">
+      <c r="F52" s="11">
         <v>246</v>
       </c>
-      <c r="G55" s="13" t="s">
+      <c r="G52" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H55" s="15">
+      <c r="H52" s="13">
         <v>32568</v>
       </c>
-      <c r="I55" s="13" t="str">
+      <c r="I52" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Maria J Pontes</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B56" s="13" t="s">
+      <c r="C53" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="C56" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="D56" s="13" t="s">
+      <c r="D53" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="E56" s="13">
+      <c r="E53" s="11">
         <v>8</v>
       </c>
-      <c r="F56" s="13">
+      <c r="F53" s="11">
         <v>100</v>
       </c>
-      <c r="G56" s="13" t="s">
+      <c r="G53" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H56" s="15">
+      <c r="H53" s="13">
         <v>33996</v>
       </c>
-      <c r="I56" s="13" t="str">
+      <c r="I53" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Anabela R Publisher</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B54" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="C54" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D54" s="11" t="s">
         <v>186</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="E57" s="13">
+      <c r="E54" s="11">
         <v>9</v>
       </c>
-      <c r="F57" s="13">
-        <v>75</v>
-      </c>
-      <c r="G57" s="13" t="s">
+      <c r="F54" s="11">
+        <v>77</v>
+      </c>
+      <c r="G54" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H57" s="15">
+      <c r="H54" s="13">
         <v>33639</v>
       </c>
-      <c r="I57" s="13" t="str">
+      <c r="I54" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Martine  Rance</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="11" t="s">
+        <v>187</v>
+      </c>
+      <c r="B55" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="C55" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="D55" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="D58" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="E58" s="13">
+      <c r="E55" s="11">
         <v>6</v>
       </c>
-      <c r="F58" s="13">
+      <c r="F55" s="11">
         <v>192</v>
       </c>
-      <c r="G58" s="13" t="s">
+      <c r="G55" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H58" s="15">
+      <c r="H55" s="13">
         <v>33588</v>
       </c>
-      <c r="I58" s="13" t="str">
+      <c r="I55" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Diego W Roel</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="13" t="s">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="B56" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="C56" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="D56" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="C59" s="13"/>
-      <c r="D59" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="E59" s="13">
+      <c r="E56" s="11">
         <v>6</v>
       </c>
-      <c r="F59" s="13">
+      <c r="F56" s="11">
         <v>152</v>
       </c>
-      <c r="G59" s="13" t="s">
+      <c r="G56" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H59" s="15">
+      <c r="H56" s="13">
         <v>32925</v>
       </c>
-      <c r="I59" s="13" t="str">
+      <c r="I56" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Annette  Roulet</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="13" t="s">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="11" t="s">
+        <v>194</v>
+      </c>
+      <c r="B57" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="C57" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D57" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="C60" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="D60" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="E60" s="13">
+      <c r="E57" s="11">
         <v>8</v>
       </c>
-      <c r="F60" s="13">
+      <c r="F57" s="11">
         <v>175</v>
       </c>
-      <c r="G60" s="13" t="s">
+      <c r="G57" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H60" s="15">
+      <c r="H57" s="13">
         <v>34149</v>
       </c>
-      <c r="I60" s="13" t="str">
+      <c r="I57" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Mary M Saveley</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="13" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B58" s="11" t="s">
         <v>198</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="C58" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D58" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="C61" s="13" t="s">
-        <v>133</v>
-      </c>
-      <c r="D61" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="E61" s="13">
+      <c r="E58" s="11">
         <v>13</v>
       </c>
-      <c r="F61" s="13">
-        <v>64</v>
-      </c>
-      <c r="G61" s="13" t="s">
+      <c r="F58" s="11">
+        <v>77</v>
+      </c>
+      <c r="G58" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H61" s="15">
+      <c r="H58" s="13">
         <v>33792</v>
       </c>
-      <c r="I61" s="13" t="str">
+      <c r="I58" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Carine G Schmitt</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="13" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="B59" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="C59" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D59" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="C62" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D62" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="E62" s="13">
+      <c r="E59" s="11">
         <v>9</v>
       </c>
-      <c r="F62" s="13">
+      <c r="F59" s="11">
         <v>78</v>
       </c>
-      <c r="G62" s="13" t="s">
+      <c r="G59" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="H62" s="15">
+      <c r="H59" s="13">
         <v>32415</v>
       </c>
-      <c r="I62" s="13" t="str">
+      <c r="I59" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Margaret A Smith</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B60" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C63" s="13" t="s">
+      <c r="C60" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D63" s="13" t="s">
+      <c r="D60" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E63" s="13">
+      <c r="E60" s="11">
         <v>12</v>
       </c>
-      <c r="F63" s="13">
+      <c r="F60" s="11">
         <v>100</v>
       </c>
-      <c r="G63" s="13" t="s">
+      <c r="G60" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H63" s="15">
+      <c r="H60" s="13">
         <v>32466</v>
       </c>
-      <c r="I63" s="13" t="str">
+      <c r="I60" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Howard A Snyder</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="13" t="s">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="B61" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="C61" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D61" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="C64" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D64" s="13" t="s">
-        <v>206</v>
-      </c>
-      <c r="E64" s="13">
+      <c r="E61" s="11">
         <v>10</v>
       </c>
-      <c r="F64" s="13">
+      <c r="F61" s="11">
         <v>165</v>
       </c>
-      <c r="G64" s="13" t="s">
+      <c r="G61" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H64" s="15">
+      <c r="H61" s="13">
         <v>32976</v>
       </c>
-      <c r="I64" s="13" t="str">
+      <c r="I61" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Martin F Sommer</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A62" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="B62" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="C62" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D62" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="C65" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="D65" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="E65" s="13">
+      <c r="E62" s="11">
         <v>9</v>
       </c>
-      <c r="F65" s="13">
+      <c r="F62" s="11">
         <v>170</v>
       </c>
-      <c r="G65" s="13" t="s">
+      <c r="G62" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="H65" s="15">
+      <c r="H62" s="13">
         <v>32364</v>
       </c>
-      <c r="I65" s="13" t="str">
+      <c r="I62" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Gary H Thomas</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="C63" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="D63" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C66" s="13" t="s">
-        <v>165</v>
-      </c>
-      <c r="D66" s="13" t="s">
-        <v>212</v>
-      </c>
-      <c r="E66" s="13">
+      <c r="E63" s="11">
         <v>11</v>
       </c>
-      <c r="F66" s="13">
-        <v>75</v>
-      </c>
-      <c r="G66" s="13" t="s">
+      <c r="F63" s="11">
+        <v>77</v>
+      </c>
+      <c r="G63" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H66" s="15">
+      <c r="H63" s="13">
         <v>32874</v>
       </c>
-      <c r="I66" s="13" t="str">
+      <c r="I63" s="11" t="str">
         <f>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</f>
         <v>Daniel B Tonini</v>
       </c>

</xml_diff>

<commit_message>
changed getDBModifDefinitions to use Workbook from Application_WorkbookActivate to avoid possible COM automation errors. Also check for names only if there is a "DBModifDef" CustomXMLParts object existing. secured setting of DBmapper ListObject in DB Modifier creation to avoid possible COM automation errors added information to exception messages to improve error retrieval improved setting of CUD Marks, fixed problem with usermsg when deletions > maxRowCountCUD setting
</commit_message>
<xml_diff>
--- a/test/DBSetQueryTests.xlsx
+++ b/test/DBSetQueryTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\DBAddin.NET\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DFBEDE4-87C1-479B-A1B8-E70EC78C9FAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8C6B42-B6ED-45C2-A93E-13860F056BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="45" windowWidth="24840" windowHeight="16545" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ConnSetting" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="42" r:id="rId5"/>
+    <pivotCache cacheId="6" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -882,15 +882,15 @@
   <dxfs count="16">
     <dxf>
       <numFmt numFmtId="20" formatCode="dd/mmm/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="20" formatCode="dd/mmm/yy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="20" formatCode="dd/mmm/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="20" formatCode="dd/mmm/yy"/>
@@ -995,7 +995,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="roland kapl" refreshedDate="45561.981961921294" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="14" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="roland kapl" refreshedDate="45569.707198842596" createdVersion="6" refreshedVersion="8" minRefreshableVersion="3" recordCount="14" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="job_id" numFmtId="0">
@@ -1158,7 +1158,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="42" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="F1:U17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisCol" showAll="0">
@@ -1408,7 +1408,7 @@
     <tableColumn id="5" xr3:uid="{A2175D36-9AE8-43F1-98C7-64AA1F79BE68}" uniqueName="5" name="job_id" queryTableFieldId="5" dataCellStyle="Standard 2"/>
     <tableColumn id="6" xr3:uid="{702F8EDC-BF8F-4491-9C31-BB133E5E74D7}" uniqueName="6" name="job_lvl" queryTableFieldId="6" dataCellStyle="Standard 2"/>
     <tableColumn id="7" xr3:uid="{12B32319-EC8F-4B98-A5B9-6546CC822FC6}" uniqueName="7" name="pub_id" queryTableFieldId="7" dataCellStyle="Standard 2"/>
-    <tableColumn id="8" xr3:uid="{ABC8CEC1-C714-4DDD-80F1-16BF0927F555}" uniqueName="8" name="hire_date" queryTableFieldId="8" dataDxfId="0" dataCellStyle="Standard 2"/>
+    <tableColumn id="8" xr3:uid="{ABC8CEC1-C714-4DDD-80F1-16BF0927F555}" uniqueName="8" name="hire_date" queryTableFieldId="8" dataDxfId="1" dataCellStyle="Standard 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1425,7 +1425,7 @@
     <tableColumn id="7" xr3:uid="{DA148D9C-ED55-4A55-A735-D448C6D4B958}" uniqueName="7" name="job_id" queryTableFieldId="6" dataDxfId="6" dataCellStyle="Standard 2"/>
     <tableColumn id="8" xr3:uid="{48381964-EB05-4B0E-97BB-10967E8923A0}" uniqueName="8" name="job_lvl" queryTableFieldId="7" dataDxfId="5" dataCellStyle="Standard 2"/>
     <tableColumn id="9" xr3:uid="{12E7DC44-9215-45EF-ACA3-923FE7BA6813}" uniqueName="9" name="pub_id" queryTableFieldId="8" dataDxfId="4" dataCellStyle="Standard 2"/>
-    <tableColumn id="10" xr3:uid="{D8BCD53C-8895-4795-AAD6-51DC52FEE94F}" uniqueName="10" name="hire_date" queryTableFieldId="9" dataDxfId="2" dataCellStyle="Standard 2"/>
+    <tableColumn id="10" xr3:uid="{D8BCD53C-8895-4795-AAD6-51DC52FEE94F}" uniqueName="10" name="hire_date" queryTableFieldId="9" dataDxfId="0" dataCellStyle="Standard 2"/>
     <tableColumn id="11" xr3:uid="{440132AD-A5A8-4107-A616-988EE8E2286F}" uniqueName="11" name="FullName" queryTableFieldId="10" dataDxfId="3" dataCellStyle="Standard 2">
       <calculatedColumnFormula>Tabelle_ExterneDaten_2[[#This Row],[fname]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[minit]]&amp;" "&amp;Tabelle_ExterneDaten_2[[#This Row],[lname]]</calculatedColumnFormula>
     </tableColumn>
@@ -1445,7 +1445,7 @@
     <tableColumn id="31" xr3:uid="{CDE367BA-72B0-4353-AA2D-14B714B22939}" uniqueName="31" name="job_id" queryTableFieldId="5" dataCellStyle="Standard 2"/>
     <tableColumn id="32" xr3:uid="{52435267-4833-407F-BEB4-7BD9095F47E5}" uniqueName="32" name="job_lvl" queryTableFieldId="6" dataCellStyle="Standard 2"/>
     <tableColumn id="33" xr3:uid="{3DDAEEAE-5D2C-4B8C-8066-B44397CD4D62}" uniqueName="33" name="pub_id" queryTableFieldId="7" dataCellStyle="Standard 2"/>
-    <tableColumn id="34" xr3:uid="{E65C2FC8-60EF-48E3-8441-EBB1B9A71822}" uniqueName="34" name="hire_date" queryTableFieldId="8" dataDxfId="1" dataCellStyle="Standard 2"/>
+    <tableColumn id="34" xr3:uid="{E65C2FC8-60EF-48E3-8441-EBB1B9A71822}" uniqueName="34" name="hire_date" queryTableFieldId="8" dataDxfId="2" dataCellStyle="Standard 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1751,7 +1751,7 @@
   <sheetPr codeName="ConnSetting"/>
   <dimension ref="A1:K1233"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -2109,8 +2109,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2250,34 +2250,33 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E8" s="15" t="s">
+      <c r="E8" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" t="s">
         <v>5</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="E9" s="15" t="s">
+      <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" t="s">
         <v>2</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15" t="s">
+      <c r="I9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2295,7 +2294,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2772,7 +2771,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2857,7 +2856,7 @@
         <v>60</v>
       </c>
       <c r="B2" s="11" t="str">
-        <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A2,"%"),"",Tabelle_ExterneDaten_1[[#Headers],[emp_id]])</f>
+        <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A2,"%"),activeConnString,Tabelle_ExterneDaten_1[[#Headers],[emp_id]])</f>
         <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False), : select * from employee where fname like 'p%'</v>
       </c>
     </row>
@@ -3129,7 +3128,7 @@
         <v>218</v>
       </c>
       <c r="B15" s="11" t="str">
-        <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A15,"%"),"",Tabelle_ExterneDaten_15[#Headers])</f>
+        <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A15,"%"),activeConnString,Tabelle_ExterneDaten_15[#Headers])</f>
         <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False), : select * from employee where fname like 'f%'</v>
       </c>
     </row>
@@ -3185,7 +3184,7 @@
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="11" t="str">
-        <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A19,"%"),"",testUnderlyingName)</f>
+        <f>_xll.DBSetQuery("select * from employee where fname like "&amp;_xll.DBString(A19,"%"),activeConnString,testUnderlyingName)</f>
         <v>Env:MSSQL, (last result:)Set OLEDB; ListObject to (bgQuery= False), : select * from employee where fname like '%'</v>
       </c>
     </row>

</xml_diff>